<commit_message>
update supplementary table 7
</commit_message>
<xml_diff>
--- a/dnam-clocks/mFSS-clock/data/processed/tables/Supplementary_table_7_IR-mFSS_genes.xlsx
+++ b/dnam-clocks/mFSS-clock/data/processed/tables/Supplementary_table_7_IR-mFSS_genes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colin\Desktop\Epigenetics paper\FSWclock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colin\Desktop\conboy-laboratory\dnam-clocks\mFSS-clock\data\processed\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE94F7E-3A4C-498C-9489-7F69A34A402C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6876BE12-42ED-456E-8E6C-AF67028FF794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="98">
   <si>
     <t>Probes</t>
   </si>
@@ -307,10 +307,13 @@
     <t>pH regulation</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
     <t xml:space="preserve">Stem cell maintenance and cancer progression </t>
+  </si>
+  <si>
+    <t>Psuedogene predicted to be involved in methylation</t>
+  </si>
+  <si>
+    <t>Chromatin remodeling</t>
   </si>
 </sst>
 </file>
@@ -685,7 +688,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1165,7 +1168,7 @@
         <v>63</v>
       </c>
       <c r="D34" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1179,7 +1182,7 @@
         <v>65</v>
       </c>
       <c r="D35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1193,7 +1196,7 @@
         <v>67</v>
       </c>
       <c r="D36" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>